<commit_message>
add info to colors in example excel skip ci
</commit_message>
<xml_diff>
--- a/data-input/example-data-input.xlsx
+++ b/data-input/example-data-input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisa/Documents/GitHub/bezirksregionenprofile-daten/data-input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55875D1A-0F01-9F4C-A404-A516942CCD50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A050D2-C438-ED49-B1C4-E787672ADE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="1300" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -892,7 +892,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1114">
   <si>
     <t>ref</t>
   </si>
@@ -4288,6 +4288,21 @@
 Die Arbeitsmappe BZR_Intro enthält Informationen zur Bezirksregion, die im oberen Teil der Detailseite (Website) angezeigt werden.
 </t>
     </r>
+  </si>
+  <si>
+    <t>#1E3791: blau</t>
+  </si>
+  <si>
+    <t>#F5F5F5</t>
+  </si>
+  <si>
+    <t>#F5F5F5: grau</t>
+  </si>
+  <si>
+    <t>#E60032: rot</t>
+  </si>
+  <si>
+    <t>Auswählbare Farbpaletten für map-pr und map-poi:</t>
   </si>
 </sst>
 </file>
@@ -4393,7 +4408,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4424,6 +4439,24 @@
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4437,7 +4470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4499,6 +4532,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5132,8 +5168,8 @@
   <dimension ref="A1:F997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -6235,7 +6271,9 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="16">
-      <c r="A69" s="19"/>
+      <c r="A69" s="19" t="s">
+        <v>1113</v>
+      </c>
       <c r="B69" s="19"/>
       <c r="C69" s="14" t="s">
         <v>159</v>
@@ -6251,7 +6289,9 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="16">
-      <c r="A70" s="19"/>
+      <c r="A70" s="36" t="s">
+        <v>1109</v>
+      </c>
       <c r="B70" s="19"/>
       <c r="C70" s="14" t="s">
         <v>161</v>
@@ -6267,7 +6307,9 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="16">
-      <c r="A71" s="19"/>
+      <c r="A71" s="35" t="s">
+        <v>1112</v>
+      </c>
       <c r="B71" s="19"/>
       <c r="C71" s="14" t="s">
         <v>164</v>
@@ -6283,7 +6325,9 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="16">
-      <c r="A72" s="19"/>
+      <c r="A72" s="37" t="s">
+        <v>1111</v>
+      </c>
       <c r="B72" s="19"/>
       <c r="C72" s="14" t="s">
         <v>166</v>
@@ -45629,7 +45673,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -45664,7 +45708,7 @@
         <v>1097</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>1056</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
update example xlsx with new pr_id's for lichtenberg skip ci
</commit_message>
<xml_diff>
--- a/data-input/example-data-input.xlsx
+++ b/data-input/example-data-input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisa/Documents/GitHub/bezirksregionenprofile-daten/data-input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A050D2-C438-ED49-B1C4-E787672ADE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF4BE55-D3E5-0D40-A3F3-36C0AA955C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="1300" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4360" yWindow="1100" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -892,7 +892,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="1132">
   <si>
     <t>ref</t>
   </si>
@@ -3609,9 +3609,6 @@
     <t>11010101</t>
   </si>
   <si>
-    <t>Dorf Malchow</t>
-  </si>
-  <si>
     <t>Malchow, Wartenberg und Falkenberg</t>
   </si>
   <si>
@@ -3621,9 +3618,6 @@
     <t>11010102</t>
   </si>
   <si>
-    <t>Dorf Wartenberg</t>
-  </si>
-  <si>
     <t>11010103</t>
   </si>
   <si>
@@ -3732,9 +3726,6 @@
     <t>11030618</t>
   </si>
   <si>
-    <t>Fennpfuhl West</t>
-  </si>
-  <si>
     <t>11030619</t>
   </si>
   <si>
@@ -3753,9 +3744,6 @@
     <t>11030721</t>
   </si>
   <si>
-    <t>Rüdigerstraße</t>
-  </si>
-  <si>
     <t>11030824</t>
   </si>
   <si>
@@ -3774,9 +3762,6 @@
     <t>11040926</t>
   </si>
   <si>
-    <t>Weitlingstraße</t>
-  </si>
-  <si>
     <t>11041022</t>
   </si>
   <si>
@@ -3799,9 +3784,6 @@
   </si>
   <si>
     <t>11041128</t>
-  </si>
-  <si>
-    <t>Sewanstraße</t>
   </si>
   <si>
     <t>Friedrichsfelde Süd</t>
@@ -4303,6 +4285,78 @@
   </si>
   <si>
     <t>Auswählbare Farbpaletten für map-pr und map-poi:</t>
+  </si>
+  <si>
+    <t>Dörfer Malchow-Wartenberg</t>
+  </si>
+  <si>
+    <t>Fennpfuhlpark</t>
+  </si>
+  <si>
+    <t>Storkower Bogen</t>
+  </si>
+  <si>
+    <t>Rudolf-Seiffert-Park</t>
+  </si>
+  <si>
+    <t>Rathaus Lichtenberg</t>
+  </si>
+  <si>
+    <t>Bornitzstraße</t>
+  </si>
+  <si>
+    <t>Roedeliusplatz</t>
+  </si>
+  <si>
+    <t>Nibelungenviertel</t>
+  </si>
+  <si>
+    <t>Nölderplatz</t>
+  </si>
+  <si>
+    <t>Weitlingkiez</t>
+  </si>
+  <si>
+    <t>Zachertstraße</t>
+  </si>
+  <si>
+    <t>Massower Straße</t>
+  </si>
+  <si>
+    <t>Dolgenseestraße</t>
+  </si>
+  <si>
+    <t>Volkradstraße</t>
+  </si>
+  <si>
+    <t>Erieseering</t>
+  </si>
+  <si>
+    <t>11051333</t>
+  </si>
+  <si>
+    <t>11051334</t>
+  </si>
+  <si>
+    <t>11051335</t>
+  </si>
+  <si>
+    <t>11051336</t>
+  </si>
+  <si>
+    <t>11051337</t>
+  </si>
+  <si>
+    <t>11051338</t>
+  </si>
+  <si>
+    <t>11051339</t>
+  </si>
+  <si>
+    <t>11051340</t>
+  </si>
+  <si>
+    <t>11051341</t>
   </si>
 </sst>
 </file>
@@ -5165,11 +5219,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F997"/>
+  <dimension ref="A1:F1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
+      <pane ySplit="1" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E440" sqref="E440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -5200,7 +5254,7 @@
     </row>
     <row r="2" spans="1:6" ht="409" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="9"/>
@@ -5210,7 +5264,7 @@
     </row>
     <row r="3" spans="1:6" ht="17">
       <c r="A3" s="33" t="s">
-        <v>1107</v>
+        <v>1101</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="14"/>
@@ -6272,7 +6326,7 @@
     </row>
     <row r="69" spans="1:6" ht="16">
       <c r="A69" s="19" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
       <c r="B69" s="19"/>
       <c r="C69" s="14" t="s">
@@ -6290,7 +6344,7 @@
     </row>
     <row r="70" spans="1:6" ht="16">
       <c r="A70" s="36" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
       <c r="B70" s="19"/>
       <c r="C70" s="14" t="s">
@@ -6308,7 +6362,7 @@
     </row>
     <row r="71" spans="1:6" ht="16">
       <c r="A71" s="35" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
       <c r="B71" s="19"/>
       <c r="C71" s="14" t="s">
@@ -6326,7 +6380,7 @@
     </row>
     <row r="72" spans="1:6" ht="16">
       <c r="A72" s="37" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
       <c r="B72" s="19"/>
       <c r="C72" s="14" t="s">
@@ -11533,1062 +11587,1113 @@
         <v>904</v>
       </c>
       <c r="D397" s="15" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E397" s="15" t="s">
         <v>905</v>
       </c>
-      <c r="E397" s="15" t="s">
+      <c r="F397" s="15" t="s">
         <v>906</v>
-      </c>
-      <c r="F397" s="15" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="398" spans="1:6" ht="16">
       <c r="A398" s="19"/>
       <c r="B398" s="19"/>
       <c r="C398" s="14" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D398" s="15" t="s">
         <v>909</v>
       </c>
       <c r="E398" s="15" t="s">
+        <v>905</v>
+      </c>
+      <c r="F398" s="15" t="s">
         <v>906</v>
-      </c>
-      <c r="F398" s="15" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="399" spans="1:6" ht="16">
       <c r="A399" s="19"/>
       <c r="B399" s="19"/>
       <c r="C399" s="14" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D399" s="15" t="s">
         <v>911</v>
       </c>
       <c r="E399" s="15" t="s">
+        <v>905</v>
+      </c>
+      <c r="F399" s="15" t="s">
         <v>906</v>
-      </c>
-      <c r="F399" s="15" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="400" spans="1:6" ht="16">
       <c r="A400" s="19"/>
       <c r="B400" s="19"/>
       <c r="C400" s="14" t="s">
+        <v>910</v>
+      </c>
+      <c r="D400" s="15" t="s">
+        <v>914</v>
+      </c>
+      <c r="E400" s="15" t="s">
         <v>912</v>
       </c>
-      <c r="D400" s="15" t="s">
-        <v>913</v>
-      </c>
-      <c r="E400" s="15" t="s">
-        <v>914</v>
-      </c>
       <c r="F400" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="401" spans="1:6" ht="16">
       <c r="A401" s="19"/>
       <c r="B401" s="19"/>
       <c r="C401" s="14" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D401" s="15" t="s">
         <v>916</v>
       </c>
       <c r="E401" s="15" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F401" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="16">
       <c r="A402" s="19"/>
       <c r="B402" s="19"/>
       <c r="C402" s="14" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D402" s="15" t="s">
         <v>918</v>
       </c>
       <c r="E402" s="15" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F402" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="403" spans="1:6" ht="16">
       <c r="A403" s="19"/>
       <c r="B403" s="19"/>
       <c r="C403" s="14" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D403" s="15" t="s">
         <v>920</v>
       </c>
       <c r="E403" s="15" t="s">
-        <v>914</v>
+        <v>921</v>
       </c>
       <c r="F403" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="404" spans="1:6" ht="16">
       <c r="A404" s="19"/>
       <c r="B404" s="19"/>
       <c r="C404" s="14" t="s">
+        <v>919</v>
+      </c>
+      <c r="D404" s="15" t="s">
+        <v>923</v>
+      </c>
+      <c r="E404" s="15" t="s">
         <v>921</v>
       </c>
-      <c r="D404" s="15" t="s">
-        <v>922</v>
-      </c>
-      <c r="E404" s="15" t="s">
-        <v>923</v>
-      </c>
       <c r="F404" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="405" spans="1:6" ht="16">
       <c r="A405" s="19"/>
       <c r="B405" s="19"/>
       <c r="C405" s="14" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D405" s="15" t="s">
         <v>925</v>
       </c>
       <c r="E405" s="15" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="F405" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="406" spans="1:6" ht="16">
       <c r="A406" s="19"/>
       <c r="B406" s="19"/>
       <c r="C406" s="14" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="D406" s="15" t="s">
         <v>927</v>
       </c>
       <c r="E406" s="15" t="s">
-        <v>923</v>
+        <v>928</v>
       </c>
       <c r="F406" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="407" spans="1:6" ht="16">
       <c r="A407" s="19"/>
       <c r="B407" s="19"/>
       <c r="C407" s="14" t="s">
+        <v>926</v>
+      </c>
+      <c r="D407" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="E407" s="15" t="s">
         <v>928</v>
       </c>
-      <c r="D407" s="15" t="s">
-        <v>929</v>
-      </c>
-      <c r="E407" s="15" t="s">
-        <v>930</v>
-      </c>
       <c r="F407" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="408" spans="1:6" ht="16">
       <c r="A408" s="19"/>
       <c r="B408" s="19"/>
       <c r="C408" s="14" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D408" s="15" t="s">
         <v>932</v>
       </c>
       <c r="E408" s="15" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
       <c r="F408" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="409" spans="1:6" ht="16">
       <c r="A409" s="19"/>
       <c r="B409" s="19"/>
       <c r="C409" s="14" t="s">
+        <v>931</v>
+      </c>
+      <c r="D409" s="15" t="s">
+        <v>935</v>
+      </c>
+      <c r="E409" s="15" t="s">
         <v>933</v>
       </c>
-      <c r="D409" s="15" t="s">
-        <v>934</v>
-      </c>
-      <c r="E409" s="15" t="s">
-        <v>935</v>
-      </c>
       <c r="F409" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="410" spans="1:6" ht="16">
       <c r="A410" s="19"/>
       <c r="B410" s="19"/>
       <c r="C410" s="14" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="D410" s="15" t="s">
         <v>937</v>
       </c>
       <c r="E410" s="15" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="F410" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="411" spans="1:6" ht="16">
       <c r="A411" s="19"/>
       <c r="B411" s="19"/>
       <c r="C411" s="14" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="D411" s="15" t="s">
         <v>939</v>
       </c>
       <c r="E411" s="15" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="F411" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="412" spans="1:6" ht="16">
       <c r="A412" s="19"/>
       <c r="B412" s="19"/>
       <c r="C412" s="14" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="D412" s="15" t="s">
         <v>941</v>
       </c>
       <c r="E412" s="15" t="s">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="F412" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="413" spans="1:6" ht="16">
       <c r="A413" s="19"/>
       <c r="B413" s="19"/>
       <c r="C413" s="14" t="s">
+        <v>940</v>
+      </c>
+      <c r="D413" s="15" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E413" s="15" t="s">
         <v>942</v>
-      </c>
-      <c r="D413" s="15" t="s">
-        <v>943</v>
-      </c>
-      <c r="E413" s="15" t="s">
-        <v>944</v>
-      </c>
-      <c r="F413" s="15" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="414" spans="1:6" ht="16">
       <c r="A414" s="19"/>
       <c r="B414" s="19"/>
       <c r="C414" s="14" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D414" s="15" t="s">
-        <v>946</v>
+        <v>1110</v>
       </c>
       <c r="E414" s="15" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="F414" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="415" spans="1:6" ht="16">
       <c r="A415" s="19"/>
       <c r="B415" s="19"/>
       <c r="C415" s="14" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="D415" s="15" t="s">
-        <v>948</v>
+        <v>1111</v>
       </c>
       <c r="E415" s="15" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="F415" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="416" spans="1:6" ht="16">
       <c r="A416" s="19"/>
       <c r="B416" s="19"/>
       <c r="C416" s="14" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="D416" s="15" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
       <c r="E416" s="15" t="s">
-        <v>951</v>
+        <v>942</v>
       </c>
       <c r="F416" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="417" spans="1:6" ht="16">
       <c r="A417" s="19"/>
       <c r="B417" s="19"/>
       <c r="C417" s="14" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="D417" s="15" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="E417" s="15" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="F417" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="418" spans="1:6" ht="16">
       <c r="A418" s="19"/>
       <c r="B418" s="19"/>
       <c r="C418" s="14" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="D418" s="15" t="s">
-        <v>955</v>
+        <v>1112</v>
       </c>
       <c r="E418" s="15" t="s">
-        <v>955</v>
+        <v>948</v>
       </c>
       <c r="F418" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="419" spans="1:6" ht="16">
       <c r="A419" s="19"/>
       <c r="B419" s="19"/>
       <c r="C419" s="14" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="D419" s="15" t="s">
-        <v>957</v>
+        <v>1113</v>
       </c>
       <c r="E419" s="15" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="F419" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="420" spans="1:6" ht="16">
       <c r="A420" s="19"/>
       <c r="B420" s="19"/>
       <c r="C420" s="14" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="D420" s="15" t="s">
-        <v>960</v>
+        <v>1114</v>
       </c>
       <c r="E420" s="15" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="F420" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="421" spans="1:6" ht="16">
       <c r="A421" s="19"/>
       <c r="B421" s="19"/>
       <c r="C421" s="14" t="s">
-        <v>961</v>
+        <v>956</v>
       </c>
       <c r="D421" s="15" t="s">
-        <v>962</v>
+        <v>1115</v>
       </c>
       <c r="E421" s="15" t="s">
-        <v>963</v>
+        <v>948</v>
       </c>
       <c r="F421" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="422" spans="1:6" ht="16">
       <c r="A422" s="19"/>
       <c r="B422" s="19"/>
       <c r="C422" s="14" t="s">
-        <v>964</v>
+        <v>959</v>
       </c>
       <c r="D422" s="15" t="s">
-        <v>965</v>
+        <v>951</v>
       </c>
       <c r="E422" s="15" t="s">
-        <v>963</v>
+        <v>175</v>
       </c>
       <c r="F422" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="423" spans="1:6" ht="16">
       <c r="A423" s="19"/>
       <c r="B423" s="19"/>
       <c r="C423" s="14" t="s">
-        <v>966</v>
+        <v>961</v>
       </c>
       <c r="D423" s="15" t="s">
-        <v>967</v>
+        <v>953</v>
       </c>
       <c r="E423" s="15" t="s">
-        <v>963</v>
+        <v>954</v>
       </c>
       <c r="F423" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="424" spans="1:6" ht="16">
       <c r="A424" s="19"/>
       <c r="B424" s="19"/>
       <c r="C424" s="14" t="s">
-        <v>968</v>
+        <v>963</v>
       </c>
       <c r="D424" s="15" t="s">
-        <v>969</v>
+        <v>1116</v>
       </c>
       <c r="E424" s="15" t="s">
-        <v>970</v>
+        <v>954</v>
       </c>
       <c r="F424" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="425" spans="1:6" ht="16">
       <c r="A425" s="19"/>
       <c r="B425" s="19"/>
       <c r="C425" s="14" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="D425" s="15" t="s">
-        <v>972</v>
+        <v>1117</v>
       </c>
       <c r="E425" s="15" t="s">
-        <v>973</v>
+        <v>954</v>
       </c>
       <c r="F425" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="426" spans="1:6" ht="16">
       <c r="A426" s="19"/>
       <c r="B426" s="19"/>
       <c r="C426" s="14" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
       <c r="D426" s="15" t="s">
-        <v>975</v>
+        <v>1118</v>
       </c>
       <c r="E426" s="15" t="s">
-        <v>976</v>
+        <v>954</v>
       </c>
       <c r="F426" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="427" spans="1:6" ht="16">
       <c r="A427" s="19"/>
       <c r="B427" s="19"/>
       <c r="C427" s="14" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="D427" s="15" t="s">
-        <v>978</v>
+        <v>1119</v>
       </c>
       <c r="E427" s="15" t="s">
-        <v>976</v>
+        <v>954</v>
       </c>
       <c r="F427" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="428" spans="1:6" ht="16">
       <c r="A428" s="19"/>
       <c r="B428" s="19"/>
       <c r="C428" s="14" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
       <c r="D428" s="15" t="s">
-        <v>980</v>
+        <v>957</v>
       </c>
       <c r="E428" s="15" t="s">
-        <v>976</v>
-      </c>
-      <c r="F428" s="15" t="s">
-        <v>907</v>
-      </c>
+        <v>958</v>
+      </c>
+      <c r="F428" s="15"/>
     </row>
     <row r="429" spans="1:6" ht="16">
       <c r="A429" s="19"/>
       <c r="B429" s="19"/>
       <c r="C429" s="14" t="s">
-        <v>981</v>
+        <v>1123</v>
       </c>
       <c r="D429" s="15" t="s">
-        <v>982</v>
+        <v>960</v>
       </c>
       <c r="E429" s="15" t="s">
-        <v>983</v>
-      </c>
-      <c r="F429" s="15" t="s">
-        <v>984</v>
-      </c>
+        <v>958</v>
+      </c>
+      <c r="F429" s="15"/>
     </row>
     <row r="430" spans="1:6" ht="16">
       <c r="A430" s="19"/>
       <c r="B430" s="19"/>
       <c r="C430" s="14" t="s">
-        <v>985</v>
+        <v>1124</v>
       </c>
       <c r="D430" s="15" t="s">
-        <v>986</v>
+        <v>962</v>
       </c>
       <c r="E430" s="15" t="s">
-        <v>983</v>
-      </c>
-      <c r="F430" s="15" t="s">
-        <v>984</v>
-      </c>
+        <v>958</v>
+      </c>
+      <c r="F430" s="15"/>
     </row>
     <row r="431" spans="1:6" ht="16">
       <c r="A431" s="19"/>
       <c r="B431" s="19"/>
       <c r="C431" s="14" t="s">
-        <v>987</v>
+        <v>1125</v>
       </c>
       <c r="D431" s="15" t="s">
-        <v>988</v>
+        <v>1120</v>
       </c>
       <c r="E431" s="15" t="s">
-        <v>983</v>
-      </c>
-      <c r="F431" s="15" t="s">
-        <v>984</v>
-      </c>
+        <v>964</v>
+      </c>
+      <c r="F431" s="15"/>
     </row>
     <row r="432" spans="1:6" ht="16">
       <c r="A432" s="19"/>
       <c r="B432" s="19"/>
       <c r="C432" s="14" t="s">
-        <v>989</v>
+        <v>1126</v>
       </c>
       <c r="D432" s="15" t="s">
-        <v>990</v>
+        <v>1121</v>
       </c>
       <c r="E432" s="15" t="s">
-        <v>991</v>
-      </c>
-      <c r="F432" s="15" t="s">
-        <v>984</v>
-      </c>
+        <v>964</v>
+      </c>
+      <c r="F432" s="15"/>
     </row>
     <row r="433" spans="1:6" ht="16">
       <c r="A433" s="19"/>
       <c r="B433" s="19"/>
       <c r="C433" s="14" t="s">
-        <v>992</v>
+        <v>1127</v>
       </c>
       <c r="D433" s="15" t="s">
-        <v>993</v>
+        <v>1122</v>
       </c>
       <c r="E433" s="15" t="s">
-        <v>991</v>
-      </c>
-      <c r="F433" s="15" t="s">
-        <v>984</v>
-      </c>
+        <v>964</v>
+      </c>
+      <c r="F433" s="15"/>
     </row>
     <row r="434" spans="1:6" ht="16">
       <c r="A434" s="19"/>
       <c r="B434" s="19"/>
       <c r="C434" s="14" t="s">
-        <v>994</v>
+        <v>1128</v>
       </c>
       <c r="D434" s="15" t="s">
-        <v>995</v>
+        <v>966</v>
       </c>
       <c r="E434" s="15" t="s">
-        <v>991</v>
-      </c>
-      <c r="F434" s="15" t="s">
-        <v>984</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="F434" s="15"/>
     </row>
     <row r="435" spans="1:6" ht="16">
       <c r="A435" s="19"/>
       <c r="B435" s="19"/>
       <c r="C435" s="14" t="s">
-        <v>996</v>
+        <v>1129</v>
       </c>
       <c r="D435" s="15" t="s">
-        <v>997</v>
+        <v>969</v>
       </c>
       <c r="E435" s="15" t="s">
-        <v>998</v>
-      </c>
-      <c r="F435" s="15" t="s">
-        <v>984</v>
-      </c>
+        <v>970</v>
+      </c>
+      <c r="F435" s="15"/>
     </row>
     <row r="436" spans="1:6" ht="16">
       <c r="A436" s="19"/>
       <c r="B436" s="19"/>
       <c r="C436" s="14" t="s">
-        <v>999</v>
+        <v>1130</v>
       </c>
       <c r="D436" s="15" t="s">
-        <v>1000</v>
+        <v>972</v>
       </c>
       <c r="E436" s="15" t="s">
-        <v>998</v>
-      </c>
-      <c r="F436" s="15" t="s">
-        <v>984</v>
-      </c>
+        <v>970</v>
+      </c>
+      <c r="F436" s="15"/>
     </row>
     <row r="437" spans="1:6" ht="16">
       <c r="A437" s="19"/>
       <c r="B437" s="19"/>
       <c r="C437" s="14" t="s">
-        <v>1001</v>
+        <v>1131</v>
       </c>
       <c r="D437" s="15" t="s">
-        <v>1002</v>
+        <v>974</v>
       </c>
       <c r="E437" s="15" t="s">
-        <v>1003</v>
+        <v>970</v>
       </c>
       <c r="F437" s="15" t="s">
-        <v>984</v>
+        <v>906</v>
       </c>
     </row>
     <row r="438" spans="1:6" ht="16">
       <c r="A438" s="19"/>
       <c r="B438" s="19"/>
       <c r="C438" s="14" t="s">
-        <v>1004</v>
+        <v>975</v>
       </c>
       <c r="D438" s="15" t="s">
-        <v>1005</v>
+        <v>976</v>
       </c>
       <c r="E438" s="15" t="s">
-        <v>1003</v>
+        <v>977</v>
       </c>
       <c r="F438" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="439" spans="1:6" ht="16">
       <c r="A439" s="19"/>
       <c r="B439" s="19"/>
       <c r="C439" s="14" t="s">
-        <v>1006</v>
+        <v>979</v>
       </c>
       <c r="D439" s="15" t="s">
-        <v>1007</v>
+        <v>980</v>
       </c>
       <c r="E439" s="15" t="s">
-        <v>1003</v>
+        <v>977</v>
       </c>
       <c r="F439" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="440" spans="1:6" ht="16">
       <c r="A440" s="19"/>
       <c r="B440" s="19"/>
       <c r="C440" s="14" t="s">
-        <v>1008</v>
+        <v>981</v>
       </c>
       <c r="D440" s="15" t="s">
-        <v>1009</v>
+        <v>982</v>
       </c>
       <c r="E440" s="15" t="s">
-        <v>1003</v>
+        <v>977</v>
       </c>
       <c r="F440" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="441" spans="1:6" ht="16">
       <c r="A441" s="19"/>
       <c r="B441" s="19"/>
       <c r="C441" s="14" t="s">
-        <v>1010</v>
+        <v>983</v>
       </c>
       <c r="D441" s="15" t="s">
-        <v>1011</v>
+        <v>984</v>
       </c>
       <c r="E441" s="15" t="s">
-        <v>1012</v>
+        <v>985</v>
       </c>
       <c r="F441" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="442" spans="1:6" ht="16">
       <c r="A442" s="19"/>
       <c r="B442" s="19"/>
       <c r="C442" s="14" t="s">
-        <v>1013</v>
+        <v>986</v>
       </c>
       <c r="D442" s="15" t="s">
-        <v>1014</v>
+        <v>987</v>
       </c>
       <c r="E442" s="15" t="s">
-        <v>1012</v>
+        <v>985</v>
       </c>
       <c r="F442" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="443" spans="1:6" ht="16">
       <c r="A443" s="19"/>
       <c r="B443" s="19"/>
       <c r="C443" s="14" t="s">
-        <v>1015</v>
+        <v>988</v>
       </c>
       <c r="D443" s="15" t="s">
-        <v>1016</v>
+        <v>989</v>
       </c>
       <c r="E443" s="15" t="s">
-        <v>1017</v>
+        <v>985</v>
       </c>
       <c r="F443" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="444" spans="1:6" ht="16">
       <c r="A444" s="19"/>
       <c r="B444" s="19"/>
       <c r="C444" s="14" t="s">
-        <v>1018</v>
+        <v>990</v>
       </c>
       <c r="D444" s="15" t="s">
-        <v>1019</v>
+        <v>991</v>
       </c>
       <c r="E444" s="15" t="s">
-        <v>1017</v>
+        <v>992</v>
       </c>
       <c r="F444" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="445" spans="1:6" ht="16">
       <c r="A445" s="19"/>
       <c r="B445" s="19"/>
       <c r="C445" s="14" t="s">
-        <v>1020</v>
+        <v>993</v>
       </c>
       <c r="D445" s="15" t="s">
-        <v>1021</v>
+        <v>994</v>
       </c>
       <c r="E445" s="15" t="s">
-        <v>1022</v>
+        <v>992</v>
       </c>
       <c r="F445" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="446" spans="1:6" ht="16">
       <c r="A446" s="19"/>
       <c r="B446" s="19"/>
       <c r="C446" s="14" t="s">
-        <v>1023</v>
+        <v>995</v>
       </c>
       <c r="D446" s="15" t="s">
-        <v>1024</v>
+        <v>996</v>
       </c>
       <c r="E446" s="15" t="s">
-        <v>1022</v>
+        <v>997</v>
       </c>
       <c r="F446" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="447" spans="1:6" ht="16">
       <c r="A447" s="19"/>
       <c r="B447" s="19"/>
       <c r="C447" s="14" t="s">
-        <v>1025</v>
+        <v>998</v>
       </c>
       <c r="D447" s="15" t="s">
-        <v>1026</v>
+        <v>999</v>
       </c>
       <c r="E447" s="15" t="s">
-        <v>1027</v>
+        <v>997</v>
       </c>
       <c r="F447" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="448" spans="1:6" ht="16">
       <c r="A448" s="19"/>
       <c r="B448" s="19"/>
       <c r="C448" s="14" t="s">
-        <v>1028</v>
+        <v>1000</v>
       </c>
       <c r="D448" s="15" t="s">
-        <v>1029</v>
+        <v>1001</v>
       </c>
       <c r="E448" s="15" t="s">
-        <v>1027</v>
+        <v>997</v>
       </c>
       <c r="F448" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="449" spans="1:6" ht="16">
       <c r="A449" s="19"/>
       <c r="B449" s="19"/>
       <c r="C449" s="14" t="s">
-        <v>1030</v>
+        <v>1002</v>
       </c>
       <c r="D449" s="15" t="s">
-        <v>1031</v>
+        <v>1003</v>
       </c>
       <c r="E449" s="15" t="s">
-        <v>1027</v>
+        <v>997</v>
       </c>
       <c r="F449" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="450" spans="1:6" ht="16">
       <c r="A450" s="19"/>
       <c r="B450" s="19"/>
       <c r="C450" s="14" t="s">
-        <v>1032</v>
+        <v>1004</v>
       </c>
       <c r="D450" s="15" t="s">
-        <v>1033</v>
+        <v>1005</v>
       </c>
       <c r="E450" s="15" t="s">
-        <v>1027</v>
+        <v>1006</v>
       </c>
       <c r="F450" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="451" spans="1:6" ht="16">
       <c r="A451" s="19"/>
       <c r="B451" s="19"/>
       <c r="C451" s="14" t="s">
-        <v>1034</v>
+        <v>1007</v>
       </c>
       <c r="D451" s="15" t="s">
-        <v>1035</v>
+        <v>1008</v>
       </c>
       <c r="E451" s="15" t="s">
-        <v>1036</v>
+        <v>1006</v>
       </c>
       <c r="F451" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="452" spans="1:6" ht="16">
       <c r="A452" s="19"/>
       <c r="B452" s="19"/>
       <c r="C452" s="14" t="s">
-        <v>1037</v>
+        <v>1009</v>
       </c>
       <c r="D452" s="15" t="s">
-        <v>1038</v>
+        <v>1010</v>
       </c>
       <c r="E452" s="15" t="s">
-        <v>1036</v>
+        <v>1011</v>
       </c>
       <c r="F452" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="453" spans="1:6" ht="16">
       <c r="A453" s="19"/>
       <c r="B453" s="19"/>
       <c r="C453" s="14" t="s">
-        <v>1039</v>
+        <v>1012</v>
       </c>
       <c r="D453" s="15" t="s">
-        <v>1040</v>
+        <v>1013</v>
       </c>
       <c r="E453" s="15" t="s">
-        <v>1036</v>
+        <v>1011</v>
       </c>
       <c r="F453" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="454" spans="1:6" ht="16">
       <c r="A454" s="19"/>
       <c r="B454" s="19"/>
       <c r="C454" s="14" t="s">
-        <v>1041</v>
+        <v>1014</v>
       </c>
       <c r="D454" s="15" t="s">
-        <v>1042</v>
+        <v>1015</v>
       </c>
       <c r="E454" s="15" t="s">
-        <v>1036</v>
+        <v>1016</v>
       </c>
       <c r="F454" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="455" spans="1:6" ht="16">
       <c r="A455" s="19"/>
       <c r="B455" s="19"/>
       <c r="C455" s="14" t="s">
-        <v>1043</v>
+        <v>1017</v>
       </c>
       <c r="D455" s="15" t="s">
-        <v>1044</v>
+        <v>1018</v>
       </c>
       <c r="E455" s="15" t="s">
-        <v>1045</v>
+        <v>1016</v>
       </c>
       <c r="F455" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="456" spans="1:6" ht="16">
       <c r="A456" s="19"/>
       <c r="B456" s="19"/>
       <c r="C456" s="14" t="s">
-        <v>1046</v>
+        <v>1019</v>
       </c>
       <c r="D456" s="15" t="s">
-        <v>1047</v>
+        <v>1020</v>
       </c>
       <c r="E456" s="15" t="s">
-        <v>1045</v>
+        <v>1021</v>
       </c>
       <c r="F456" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="457" spans="1:6" ht="16">
       <c r="A457" s="19"/>
       <c r="B457" s="19"/>
       <c r="C457" s="14" t="s">
-        <v>1048</v>
+        <v>1022</v>
       </c>
       <c r="D457" s="15" t="s">
-        <v>1049</v>
+        <v>1023</v>
       </c>
       <c r="E457" s="15" t="s">
-        <v>1050</v>
+        <v>1021</v>
       </c>
       <c r="F457" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="458" spans="1:6" ht="16">
       <c r="A458" s="19"/>
       <c r="B458" s="19"/>
       <c r="C458" s="14" t="s">
-        <v>1051</v>
+        <v>1024</v>
       </c>
       <c r="D458" s="15" t="s">
-        <v>1052</v>
+        <v>1025</v>
       </c>
       <c r="E458" s="15" t="s">
-        <v>1050</v>
+        <v>1021</v>
       </c>
       <c r="F458" s="15" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
     </row>
     <row r="459" spans="1:6" ht="16">
       <c r="A459" s="19"/>
       <c r="B459" s="19"/>
-      <c r="C459" s="14"/>
-      <c r="D459" s="15"/>
-      <c r="E459" s="15"/>
-      <c r="F459" s="15"/>
+      <c r="C459" s="14" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D459" s="15" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E459" s="15" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F459" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="460" spans="1:6" ht="16">
       <c r="A460" s="19"/>
       <c r="B460" s="19"/>
-      <c r="C460" s="14"/>
-      <c r="D460" s="15"/>
-      <c r="E460" s="15"/>
-      <c r="F460" s="15"/>
+      <c r="C460" s="14" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D460" s="15" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E460" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F460" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="461" spans="1:6" ht="16">
       <c r="A461" s="19"/>
       <c r="B461" s="19"/>
-      <c r="C461" s="14"/>
-      <c r="D461" s="15"/>
-      <c r="E461" s="15"/>
-      <c r="F461" s="15"/>
+      <c r="C461" s="14" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D461" s="15" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E461" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F461" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="462" spans="1:6" ht="16">
       <c r="A462" s="19"/>
       <c r="B462" s="19"/>
-      <c r="C462" s="14"/>
-      <c r="D462" s="15"/>
-      <c r="E462" s="15"/>
-      <c r="F462" s="15"/>
+      <c r="C462" s="14" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D462" s="15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E462" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F462" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="463" spans="1:6" ht="16">
       <c r="A463" s="19"/>
       <c r="B463" s="19"/>
-      <c r="C463" s="14"/>
-      <c r="D463" s="15"/>
-      <c r="E463" s="15"/>
-      <c r="F463" s="15"/>
+      <c r="C463" s="14" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D463" s="15" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E463" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F463" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="464" spans="1:6" ht="16">
       <c r="A464" s="19"/>
       <c r="B464" s="19"/>
-      <c r="C464" s="14"/>
-      <c r="D464" s="15"/>
-      <c r="E464" s="15"/>
-      <c r="F464" s="15"/>
+      <c r="C464" s="14" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D464" s="15" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E464" s="15" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F464" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="465" spans="1:6" ht="16">
       <c r="A465" s="19"/>
       <c r="B465" s="19"/>
-      <c r="C465" s="14"/>
-      <c r="D465" s="15"/>
-      <c r="E465" s="15"/>
-      <c r="F465" s="15"/>
+      <c r="C465" s="14" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D465" s="15" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E465" s="15" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F465" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="466" spans="1:6" ht="16">
       <c r="A466" s="19"/>
       <c r="B466" s="19"/>
-      <c r="C466" s="14"/>
-      <c r="D466" s="15"/>
-      <c r="E466" s="15"/>
-      <c r="F466" s="15"/>
+      <c r="C466" s="14" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D466" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E466" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F466" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="467" spans="1:6" ht="16">
       <c r="A467" s="19"/>
       <c r="B467" s="19"/>
-      <c r="C467" s="14"/>
-      <c r="D467" s="15"/>
-      <c r="E467" s="15"/>
-      <c r="F467" s="15"/>
+      <c r="C467" s="14" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D467" s="15" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E467" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F467" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="468" spans="1:6" ht="16">
       <c r="A468" s="19"/>
@@ -16815,6 +16920,7 @@
       <c r="F995" s="15"/>
     </row>
     <row r="996" spans="1:6" ht="16">
+      <c r="A996" s="19"/>
       <c r="B996" s="19"/>
       <c r="C996" s="14"/>
       <c r="D996" s="15"/>
@@ -16822,11 +16928,82 @@
       <c r="F996" s="15"/>
     </row>
     <row r="997" spans="1:6" ht="16">
+      <c r="A997" s="19"/>
       <c r="B997" s="19"/>
       <c r="C997" s="14"/>
       <c r="D997" s="15"/>
       <c r="E997" s="15"/>
       <c r="F997" s="15"/>
+    </row>
+    <row r="998" spans="1:6" ht="16">
+      <c r="A998" s="19"/>
+      <c r="B998" s="19"/>
+      <c r="C998" s="14"/>
+      <c r="D998" s="15"/>
+      <c r="E998" s="15"/>
+      <c r="F998" s="15"/>
+    </row>
+    <row r="999" spans="1:6" ht="16">
+      <c r="A999" s="19"/>
+      <c r="B999" s="19"/>
+      <c r="C999" s="14"/>
+      <c r="D999" s="15"/>
+      <c r="E999" s="15"/>
+      <c r="F999" s="15"/>
+    </row>
+    <row r="1000" spans="1:6" ht="16">
+      <c r="A1000" s="19"/>
+      <c r="B1000" s="19"/>
+      <c r="C1000" s="14"/>
+      <c r="D1000" s="15"/>
+      <c r="E1000" s="15"/>
+      <c r="F1000" s="15"/>
+    </row>
+    <row r="1001" spans="1:6" ht="16">
+      <c r="A1001" s="19"/>
+      <c r="B1001" s="19"/>
+      <c r="C1001" s="14"/>
+      <c r="D1001" s="15"/>
+      <c r="E1001" s="15"/>
+      <c r="F1001" s="15"/>
+    </row>
+    <row r="1002" spans="1:6" ht="16">
+      <c r="A1002" s="19"/>
+      <c r="B1002" s="19"/>
+      <c r="C1002" s="14"/>
+      <c r="D1002" s="15"/>
+      <c r="E1002" s="15"/>
+      <c r="F1002" s="15"/>
+    </row>
+    <row r="1003" spans="1:6" ht="16">
+      <c r="A1003" s="19"/>
+      <c r="B1003" s="19"/>
+      <c r="C1003" s="14"/>
+      <c r="D1003" s="15"/>
+      <c r="E1003" s="15"/>
+      <c r="F1003" s="15"/>
+    </row>
+    <row r="1004" spans="1:6" ht="16">
+      <c r="A1004" s="19"/>
+      <c r="B1004" s="19"/>
+      <c r="C1004" s="14"/>
+      <c r="D1004" s="15"/>
+      <c r="E1004" s="15"/>
+      <c r="F1004" s="15"/>
+    </row>
+    <row r="1005" spans="1:6" ht="16">
+      <c r="B1005" s="19"/>
+      <c r="C1005" s="14"/>
+      <c r="D1005" s="15"/>
+      <c r="E1005" s="15"/>
+      <c r="F1005" s="15"/>
+    </row>
+    <row r="1006" spans="1:6" ht="16">
+      <c r="B1006" s="19"/>
+      <c r="C1006" s="14"/>
+      <c r="D1006" s="15"/>
+      <c r="E1006" s="15"/>
+      <c r="F1006" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -16865,10 +17042,10 @@
         <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -16945,10 +17122,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>1093</v>
+        <v>1087</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -17016,7 +17193,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -17051,7 +17228,7 @@
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="34" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -17085,16 +17262,16 @@
         <v>45</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -17126,16 +17303,16 @@
         <v>51</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>127</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -17166,16 +17343,16 @@
         <v>101</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>1102</v>
+        <v>1096</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>224</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -17206,16 +17383,16 @@
         <v>107</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>238</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
@@ -17250,13 +17427,13 @@
         <v>121</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -45684,16 +45861,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1067</v>
+        <v>1061</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
@@ -45705,10 +45882,10 @@
         <v>25</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
@@ -49763,53 +49940,53 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="22" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>1054</v>
+        <v>1048</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>1059</v>
+        <v>1053</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>1060</v>
+        <v>1054</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>1061</v>
+        <v>1055</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>1063</v>
+        <v>1057</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="D4" s="24"/>
     </row>
@@ -54835,22 +55012,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1069</v>
+        <v>1063</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1070</v>
+        <v>1064</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>1072</v>
+        <v>1066</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -54878,10 +55055,10 @@
         <v>2015</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="D2" s="32">
         <v>145</v>
@@ -58936,22 +59113,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1069</v>
+        <v>1063</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1070</v>
+        <v>1064</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>1072</v>
+        <v>1066</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -58976,13 +59153,13 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="32" t="s">
-        <v>1075</v>
+        <v>1069</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1076</v>
+        <v>1070</v>
       </c>
       <c r="D2" s="32">
         <v>145</v>
@@ -58996,7 +59173,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="32" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -59012,7 +59189,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="32" t="s">
-        <v>1078</v>
+        <v>1072</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -63034,19 +63211,19 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1081</v>
+        <v>1075</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1082</v>
+        <v>1076</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -63072,7 +63249,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
       <c r="B2" s="5">
         <v>4923</v>
@@ -63090,7 +63267,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
       <c r="B3" s="5">
         <v>1202</v>
@@ -63108,7 +63285,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
       <c r="B4" s="5">
         <v>3002</v>
@@ -63126,7 +63303,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>1087</v>
+        <v>1081</v>
       </c>
       <c r="B5" s="5">
         <v>1234</v>
@@ -63144,7 +63321,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
       <c r="B6" s="5">
         <v>4321</v>
@@ -63162,7 +63339,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
       <c r="B7" s="5">
         <v>3211</v>

</xml_diff>

<commit_message>
update example excel skip ci
</commit_message>
<xml_diff>
--- a/data-input/example-data-input.xlsx
+++ b/data-input/example-data-input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisa/Documents/GitHub/bezirksregionenprofile-daten/data-input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF4BE55-D3E5-0D40-A3F3-36C0AA955C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B2D1F8-4296-4747-9EE5-661B2029B762}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="1100" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -892,7 +892,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="1091">
   <si>
     <t>ref</t>
   </si>
@@ -3606,214 +3606,118 @@
     <t>Mahlsdorf Süd</t>
   </si>
   <si>
-    <t>11010101</t>
-  </si>
-  <si>
     <t>Malchow, Wartenberg und Falkenberg</t>
   </si>
   <si>
     <t>Lichtenberg</t>
   </si>
   <si>
-    <t>11010102</t>
-  </si>
-  <si>
-    <t>11010103</t>
-  </si>
-  <si>
     <t>Dorf Falkenberg</t>
   </si>
   <si>
-    <t>11010204</t>
-  </si>
-  <si>
     <t>Falkenberg Ost</t>
   </si>
   <si>
     <t>Neu-Hohenschönhausen Nord</t>
   </si>
   <si>
-    <t>11010205</t>
-  </si>
-  <si>
     <t>Falkenberg West</t>
   </si>
   <si>
-    <t>11010206</t>
-  </si>
-  <si>
     <t>Wartenberg Süd</t>
   </si>
   <si>
-    <t>11010207</t>
-  </si>
-  <si>
     <t>Wartenberg Nord</t>
   </si>
   <si>
-    <t>11010308</t>
-  </si>
-  <si>
     <t>Zingster Straße Ost</t>
   </si>
   <si>
     <t>Neu-Hohenschönhausen Süd</t>
   </si>
   <si>
-    <t>11010309</t>
-  </si>
-  <si>
     <t>Zingster Straße West</t>
   </si>
   <si>
-    <t>11010310</t>
-  </si>
-  <si>
     <t>Mühlengrund</t>
   </si>
   <si>
-    <t>11020411</t>
-  </si>
-  <si>
     <t>Malchower Weg</t>
   </si>
   <si>
     <t>Alt-Hohenschönhausen Nord</t>
   </si>
   <si>
-    <t>11020412</t>
-  </si>
-  <si>
     <t>Hauptstraße</t>
   </si>
   <si>
-    <t>11020513</t>
-  </si>
-  <si>
     <t>Orankesee</t>
   </si>
   <si>
     <t>Alt-Hohenschönhausen Süd</t>
   </si>
   <si>
-    <t>11020514</t>
-  </si>
-  <si>
     <t>Große-Leege-Straße</t>
   </si>
   <si>
-    <t>11020515</t>
-  </si>
-  <si>
     <t>Landsberger Allee</t>
   </si>
   <si>
-    <t>11020516</t>
-  </si>
-  <si>
     <t>Weiße Taube</t>
   </si>
   <si>
-    <t>11030617</t>
-  </si>
-  <si>
     <t>Hohenschönhausener Straße</t>
   </si>
   <si>
     <t>Fennpfuhl</t>
   </si>
   <si>
-    <t>11030618</t>
-  </si>
-  <si>
-    <t>11030619</t>
-  </si>
-  <si>
     <t>Fennpfuhl Ost</t>
   </si>
   <si>
-    <t>11030720</t>
-  </si>
-  <si>
     <t>Herzbergstraße</t>
   </si>
   <si>
     <t>Alt-Lichtenberg</t>
   </si>
   <si>
-    <t>11030721</t>
-  </si>
-  <si>
-    <t>11030824</t>
-  </si>
-  <si>
     <t>Frankfurter Allee Süd</t>
   </si>
   <si>
-    <t>11040925</t>
-  </si>
-  <si>
     <t>Victoriastadt</t>
   </si>
   <si>
     <t>Neu-Lichtenberg</t>
   </si>
   <si>
-    <t>11040926</t>
-  </si>
-  <si>
-    <t>11041022</t>
-  </si>
-  <si>
     <t>Rosenfelder Ring</t>
   </si>
   <si>
     <t>Friedrichsfelde Nord</t>
   </si>
   <si>
-    <t>11041023</t>
-  </si>
-  <si>
     <t>Gensinger Straße</t>
   </si>
   <si>
-    <t>11041027</t>
-  </si>
-  <si>
     <t>Tierpark</t>
   </si>
   <si>
-    <t>11041128</t>
-  </si>
-  <si>
     <t>Friedrichsfelde Süd</t>
   </si>
   <si>
-    <t>11051229</t>
-  </si>
-  <si>
     <t>Rummelsburg</t>
   </si>
   <si>
     <t>Rummelsburger Bucht</t>
   </si>
   <si>
-    <t>11051330</t>
-  </si>
-  <si>
     <t>Karlshorst West</t>
   </si>
   <si>
     <t>Karlshorst</t>
   </si>
   <si>
-    <t>11051331</t>
-  </si>
-  <si>
     <t>Karlshorst Nord</t>
-  </si>
-  <si>
-    <t>11051332</t>
   </si>
   <si>
     <t>Karlshorst Süd</t>
@@ -4330,33 +4234,6 @@
   </si>
   <si>
     <t>Erieseering</t>
-  </si>
-  <si>
-    <t>11051333</t>
-  </si>
-  <si>
-    <t>11051334</t>
-  </si>
-  <si>
-    <t>11051335</t>
-  </si>
-  <si>
-    <t>11051336</t>
-  </si>
-  <si>
-    <t>11051337</t>
-  </si>
-  <si>
-    <t>11051338</t>
-  </si>
-  <si>
-    <t>11051339</t>
-  </si>
-  <si>
-    <t>11051340</t>
-  </si>
-  <si>
-    <t>11051341</t>
   </si>
 </sst>
 </file>
@@ -5222,8 +5099,8 @@
   <dimension ref="A1:F1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E440" sqref="E440"/>
+      <pane ySplit="1" topLeftCell="A410" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D412" sqref="D412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -5254,7 +5131,7 @@
     </row>
     <row r="2" spans="1:6" ht="409" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>1102</v>
+        <v>1070</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="9"/>
@@ -5264,7 +5141,7 @@
     </row>
     <row r="3" spans="1:6" ht="17">
       <c r="A3" s="33" t="s">
-        <v>1101</v>
+        <v>1069</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="14"/>
@@ -6326,7 +6203,7 @@
     </row>
     <row r="69" spans="1:6" ht="16">
       <c r="A69" s="19" t="s">
-        <v>1107</v>
+        <v>1075</v>
       </c>
       <c r="B69" s="19"/>
       <c r="C69" s="14" t="s">
@@ -6344,7 +6221,7 @@
     </row>
     <row r="70" spans="1:6" ht="16">
       <c r="A70" s="36" t="s">
-        <v>1103</v>
+        <v>1071</v>
       </c>
       <c r="B70" s="19"/>
       <c r="C70" s="14" t="s">
@@ -6362,7 +6239,7 @@
     </row>
     <row r="71" spans="1:6" ht="16">
       <c r="A71" s="35" t="s">
-        <v>1106</v>
+        <v>1074</v>
       </c>
       <c r="B71" s="19"/>
       <c r="C71" s="14" t="s">
@@ -6380,7 +6257,7 @@
     </row>
     <row r="72" spans="1:6" ht="16">
       <c r="A72" s="37" t="s">
-        <v>1105</v>
+        <v>1073</v>
       </c>
       <c r="B72" s="19"/>
       <c r="C72" s="14" t="s">
@@ -11583,1116 +11460,1137 @@
     <row r="397" spans="1:6" ht="16">
       <c r="A397" s="19"/>
       <c r="B397" s="19"/>
-      <c r="C397" s="14" t="s">
+      <c r="C397" s="14">
+        <v>11100101</v>
+      </c>
+      <c r="D397" s="15" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E397" s="15" t="s">
         <v>904</v>
       </c>
-      <c r="D397" s="15" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E397" s="15" t="s">
+      <c r="F397" s="15" t="s">
         <v>905</v>
-      </c>
-      <c r="F397" s="15" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="398" spans="1:6" ht="16">
       <c r="A398" s="19"/>
       <c r="B398" s="19"/>
-      <c r="C398" s="14" t="s">
-        <v>907</v>
+      <c r="C398" s="14">
+        <v>11100102</v>
       </c>
       <c r="D398" s="15" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="E398" s="15" t="s">
+        <v>904</v>
+      </c>
+      <c r="F398" s="15" t="s">
         <v>905</v>
-      </c>
-      <c r="F398" s="15" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="399" spans="1:6" ht="16">
       <c r="A399" s="19"/>
       <c r="B399" s="19"/>
-      <c r="C399" s="14" t="s">
-        <v>908</v>
+      <c r="C399" s="14">
+        <v>11100203</v>
       </c>
       <c r="D399" s="15" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="E399" s="15" t="s">
+        <v>904</v>
+      </c>
+      <c r="F399" s="15" t="s">
         <v>905</v>
-      </c>
-      <c r="F399" s="15" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="400" spans="1:6" ht="16">
       <c r="A400" s="19"/>
       <c r="B400" s="19"/>
-      <c r="C400" s="14" t="s">
-        <v>910</v>
+      <c r="C400" s="14">
+        <v>11100204</v>
       </c>
       <c r="D400" s="15" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
       <c r="E400" s="15" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="F400" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="401" spans="1:6" ht="16">
       <c r="A401" s="19"/>
       <c r="B401" s="19"/>
-      <c r="C401" s="14" t="s">
-        <v>913</v>
+      <c r="C401" s="14">
+        <v>11100205</v>
       </c>
       <c r="D401" s="15" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="E401" s="15" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="F401" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="16">
       <c r="A402" s="19"/>
       <c r="B402" s="19"/>
-      <c r="C402" s="14" t="s">
-        <v>915</v>
+      <c r="C402" s="14">
+        <v>11100206</v>
       </c>
       <c r="D402" s="15" t="s">
-        <v>918</v>
+        <v>911</v>
       </c>
       <c r="E402" s="15" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="F402" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="403" spans="1:6" ht="16">
       <c r="A403" s="19"/>
       <c r="B403" s="19"/>
-      <c r="C403" s="14" t="s">
-        <v>917</v>
+      <c r="C403" s="14">
+        <v>11100307</v>
       </c>
       <c r="D403" s="15" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="E403" s="15" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="F403" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="404" spans="1:6" ht="16">
       <c r="A404" s="19"/>
       <c r="B404" s="19"/>
-      <c r="C404" s="14" t="s">
-        <v>919</v>
+      <c r="C404" s="14">
+        <v>11100308</v>
       </c>
       <c r="D404" s="15" t="s">
-        <v>923</v>
+        <v>914</v>
       </c>
       <c r="E404" s="15" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="F404" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="405" spans="1:6" ht="16">
       <c r="A405" s="19"/>
       <c r="B405" s="19"/>
-      <c r="C405" s="14" t="s">
-        <v>922</v>
+      <c r="C405" s="14">
+        <v>11100309</v>
       </c>
       <c r="D405" s="15" t="s">
-        <v>925</v>
+        <v>915</v>
       </c>
       <c r="E405" s="15" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="F405" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="406" spans="1:6" ht="16">
       <c r="A406" s="19"/>
       <c r="B406" s="19"/>
-      <c r="C406" s="14" t="s">
-        <v>924</v>
+      <c r="C406" s="14">
+        <v>11200410</v>
       </c>
       <c r="D406" s="15" t="s">
-        <v>927</v>
+        <v>916</v>
       </c>
       <c r="E406" s="15" t="s">
-        <v>928</v>
+        <v>917</v>
       </c>
       <c r="F406" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="407" spans="1:6" ht="16">
       <c r="A407" s="19"/>
       <c r="B407" s="19"/>
-      <c r="C407" s="14" t="s">
-        <v>926</v>
+      <c r="C407" s="14">
+        <v>11200411</v>
       </c>
       <c r="D407" s="15" t="s">
-        <v>930</v>
+        <v>918</v>
       </c>
       <c r="E407" s="15" t="s">
-        <v>928</v>
+        <v>917</v>
       </c>
       <c r="F407" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="408" spans="1:6" ht="16">
       <c r="A408" s="19"/>
       <c r="B408" s="19"/>
-      <c r="C408" s="14" t="s">
-        <v>929</v>
+      <c r="C408" s="14">
+        <v>11200512</v>
       </c>
       <c r="D408" s="15" t="s">
-        <v>932</v>
+        <v>919</v>
       </c>
       <c r="E408" s="15" t="s">
-        <v>933</v>
+        <v>920</v>
       </c>
       <c r="F408" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="409" spans="1:6" ht="16">
       <c r="A409" s="19"/>
       <c r="B409" s="19"/>
-      <c r="C409" s="14" t="s">
-        <v>931</v>
+      <c r="C409" s="14">
+        <v>11200513</v>
       </c>
       <c r="D409" s="15" t="s">
-        <v>935</v>
+        <v>921</v>
       </c>
       <c r="E409" s="15" t="s">
-        <v>933</v>
+        <v>920</v>
       </c>
       <c r="F409" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="410" spans="1:6" ht="16">
       <c r="A410" s="19"/>
       <c r="B410" s="19"/>
-      <c r="C410" s="14" t="s">
-        <v>934</v>
+      <c r="C410" s="14">
+        <v>11200514</v>
       </c>
       <c r="D410" s="15" t="s">
-        <v>937</v>
+        <v>922</v>
       </c>
       <c r="E410" s="15" t="s">
-        <v>933</v>
+        <v>920</v>
       </c>
       <c r="F410" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="411" spans="1:6" ht="16">
       <c r="A411" s="19"/>
       <c r="B411" s="19"/>
-      <c r="C411" s="14" t="s">
-        <v>936</v>
+      <c r="C411" s="14">
+        <v>11200515</v>
       </c>
       <c r="D411" s="15" t="s">
-        <v>939</v>
+        <v>923</v>
       </c>
       <c r="E411" s="15" t="s">
-        <v>933</v>
+        <v>920</v>
       </c>
       <c r="F411" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="412" spans="1:6" ht="16">
       <c r="A412" s="19"/>
       <c r="B412" s="19"/>
-      <c r="C412" s="14" t="s">
-        <v>938</v>
+      <c r="C412" s="14">
+        <v>11300616</v>
       </c>
       <c r="D412" s="15" t="s">
-        <v>941</v>
+        <v>924</v>
       </c>
       <c r="E412" s="15" t="s">
-        <v>942</v>
+        <v>925</v>
       </c>
       <c r="F412" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="413" spans="1:6" ht="16">
       <c r="A413" s="19"/>
       <c r="B413" s="19"/>
-      <c r="C413" s="14" t="s">
-        <v>940</v>
+      <c r="C413" s="14">
+        <v>11300617</v>
       </c>
       <c r="D413" s="15" t="s">
-        <v>1109</v>
+        <v>1077</v>
       </c>
       <c r="E413" s="15" t="s">
-        <v>942</v>
+        <v>925</v>
+      </c>
+      <c r="F413" s="15" t="s">
+        <v>905</v>
       </c>
     </row>
     <row r="414" spans="1:6" ht="16">
       <c r="A414" s="19"/>
       <c r="B414" s="19"/>
-      <c r="C414" s="14" t="s">
-        <v>943</v>
+      <c r="C414" s="14">
+        <v>11300618</v>
       </c>
       <c r="D414" s="15" t="s">
-        <v>1110</v>
+        <v>1078</v>
       </c>
       <c r="E414" s="15" t="s">
-        <v>942</v>
+        <v>925</v>
       </c>
       <c r="F414" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="415" spans="1:6" ht="16">
       <c r="A415" s="19"/>
       <c r="B415" s="19"/>
-      <c r="C415" s="14" t="s">
-        <v>944</v>
+      <c r="C415" s="14">
+        <v>11300619</v>
       </c>
       <c r="D415" s="15" t="s">
-        <v>1111</v>
+        <v>1079</v>
       </c>
       <c r="E415" s="15" t="s">
-        <v>942</v>
+        <v>925</v>
       </c>
       <c r="F415" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="416" spans="1:6" ht="16">
       <c r="A416" s="19"/>
       <c r="B416" s="19"/>
-      <c r="C416" s="14" t="s">
-        <v>946</v>
+      <c r="C416" s="14">
+        <v>11300620</v>
       </c>
       <c r="D416" s="15" t="s">
-        <v>945</v>
+        <v>926</v>
       </c>
       <c r="E416" s="15" t="s">
-        <v>942</v>
+        <v>925</v>
       </c>
       <c r="F416" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="417" spans="1:6" ht="16">
       <c r="A417" s="19"/>
       <c r="B417" s="19"/>
-      <c r="C417" s="14" t="s">
-        <v>949</v>
+      <c r="C417" s="14">
+        <v>11300721</v>
       </c>
       <c r="D417" s="15" t="s">
-        <v>947</v>
+        <v>927</v>
       </c>
       <c r="E417" s="15" t="s">
-        <v>948</v>
+        <v>928</v>
       </c>
       <c r="F417" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="418" spans="1:6" ht="16">
       <c r="A418" s="19"/>
       <c r="B418" s="19"/>
-      <c r="C418" s="14" t="s">
-        <v>950</v>
+      <c r="C418" s="14">
+        <v>11300722</v>
       </c>
       <c r="D418" s="15" t="s">
-        <v>1112</v>
+        <v>1080</v>
       </c>
       <c r="E418" s="15" t="s">
-        <v>948</v>
+        <v>928</v>
       </c>
       <c r="F418" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="419" spans="1:6" ht="16">
       <c r="A419" s="19"/>
       <c r="B419" s="19"/>
-      <c r="C419" s="14" t="s">
-        <v>952</v>
+      <c r="C419" s="14">
+        <v>11300723</v>
       </c>
       <c r="D419" s="15" t="s">
-        <v>1113</v>
+        <v>1081</v>
       </c>
       <c r="E419" s="15" t="s">
-        <v>948</v>
+        <v>928</v>
       </c>
       <c r="F419" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="420" spans="1:6" ht="16">
       <c r="A420" s="19"/>
       <c r="B420" s="19"/>
-      <c r="C420" s="14" t="s">
-        <v>955</v>
+      <c r="C420" s="14">
+        <v>11300724</v>
       </c>
       <c r="D420" s="15" t="s">
-        <v>1114</v>
+        <v>1082</v>
       </c>
       <c r="E420" s="15" t="s">
-        <v>948</v>
+        <v>928</v>
       </c>
       <c r="F420" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="421" spans="1:6" ht="16">
       <c r="A421" s="19"/>
       <c r="B421" s="19"/>
-      <c r="C421" s="14" t="s">
-        <v>956</v>
+      <c r="C421" s="14">
+        <v>11300725</v>
       </c>
       <c r="D421" s="15" t="s">
-        <v>1115</v>
+        <v>1083</v>
       </c>
       <c r="E421" s="15" t="s">
-        <v>948</v>
+        <v>928</v>
       </c>
       <c r="F421" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="422" spans="1:6" ht="16">
       <c r="A422" s="19"/>
       <c r="B422" s="19"/>
-      <c r="C422" s="14" t="s">
-        <v>959</v>
+      <c r="C422" s="14">
+        <v>11300826</v>
       </c>
       <c r="D422" s="15" t="s">
-        <v>951</v>
+        <v>929</v>
       </c>
       <c r="E422" s="15" t="s">
-        <v>175</v>
+        <v>929</v>
       </c>
       <c r="F422" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="423" spans="1:6" ht="16">
       <c r="A423" s="19"/>
       <c r="B423" s="19"/>
-      <c r="C423" s="14" t="s">
-        <v>961</v>
+      <c r="C423" s="14">
+        <v>11400927</v>
       </c>
       <c r="D423" s="15" t="s">
-        <v>953</v>
+        <v>930</v>
       </c>
       <c r="E423" s="15" t="s">
-        <v>954</v>
+        <v>931</v>
       </c>
       <c r="F423" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="424" spans="1:6" ht="16">
       <c r="A424" s="19"/>
       <c r="B424" s="19"/>
-      <c r="C424" s="14" t="s">
-        <v>963</v>
+      <c r="C424" s="14">
+        <v>11400928</v>
       </c>
       <c r="D424" s="15" t="s">
-        <v>1116</v>
+        <v>1084</v>
       </c>
       <c r="E424" s="15" t="s">
-        <v>954</v>
+        <v>931</v>
       </c>
       <c r="F424" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="425" spans="1:6" ht="16">
       <c r="A425" s="19"/>
       <c r="B425" s="19"/>
-      <c r="C425" s="14" t="s">
-        <v>965</v>
+      <c r="C425" s="14">
+        <v>11400929</v>
       </c>
       <c r="D425" s="15" t="s">
-        <v>1117</v>
+        <v>1085</v>
       </c>
       <c r="E425" s="15" t="s">
-        <v>954</v>
+        <v>931</v>
       </c>
       <c r="F425" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="426" spans="1:6" ht="16">
       <c r="A426" s="19"/>
       <c r="B426" s="19"/>
-      <c r="C426" s="14" t="s">
-        <v>968</v>
+      <c r="C426" s="14">
+        <v>11400930</v>
       </c>
       <c r="D426" s="15" t="s">
-        <v>1118</v>
+        <v>1086</v>
       </c>
       <c r="E426" s="15" t="s">
-        <v>954</v>
+        <v>931</v>
       </c>
       <c r="F426" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="427" spans="1:6" ht="16">
       <c r="A427" s="19"/>
       <c r="B427" s="19"/>
-      <c r="C427" s="14" t="s">
-        <v>971</v>
+      <c r="C427" s="14">
+        <v>11400931</v>
       </c>
       <c r="D427" s="15" t="s">
-        <v>1119</v>
+        <v>1087</v>
       </c>
       <c r="E427" s="15" t="s">
-        <v>954</v>
+        <v>931</v>
       </c>
       <c r="F427" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="428" spans="1:6" ht="16">
       <c r="A428" s="19"/>
       <c r="B428" s="19"/>
-      <c r="C428" s="14" t="s">
-        <v>973</v>
+      <c r="C428" s="14">
+        <v>11401032</v>
       </c>
       <c r="D428" s="15" t="s">
-        <v>957</v>
+        <v>932</v>
       </c>
       <c r="E428" s="15" t="s">
-        <v>958</v>
-      </c>
-      <c r="F428" s="15"/>
+        <v>933</v>
+      </c>
+      <c r="F428" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="429" spans="1:6" ht="16">
       <c r="A429" s="19"/>
       <c r="B429" s="19"/>
-      <c r="C429" s="14" t="s">
-        <v>1123</v>
+      <c r="C429" s="14">
+        <v>11401033</v>
       </c>
       <c r="D429" s="15" t="s">
-        <v>960</v>
+        <v>934</v>
       </c>
       <c r="E429" s="15" t="s">
-        <v>958</v>
-      </c>
-      <c r="F429" s="15"/>
+        <v>933</v>
+      </c>
+      <c r="F429" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="430" spans="1:6" ht="16">
       <c r="A430" s="19"/>
       <c r="B430" s="19"/>
-      <c r="C430" s="14" t="s">
-        <v>1124</v>
+      <c r="C430" s="14">
+        <v>11401034</v>
       </c>
       <c r="D430" s="15" t="s">
-        <v>962</v>
+        <v>935</v>
       </c>
       <c r="E430" s="15" t="s">
-        <v>958</v>
-      </c>
-      <c r="F430" s="15"/>
+        <v>933</v>
+      </c>
+      <c r="F430" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="431" spans="1:6" ht="16">
       <c r="A431" s="19"/>
       <c r="B431" s="19"/>
-      <c r="C431" s="14" t="s">
-        <v>1125</v>
+      <c r="C431" s="14">
+        <v>11401135</v>
       </c>
       <c r="D431" s="15" t="s">
-        <v>1120</v>
+        <v>1088</v>
       </c>
       <c r="E431" s="15" t="s">
-        <v>964</v>
-      </c>
-      <c r="F431" s="15"/>
+        <v>936</v>
+      </c>
+      <c r="F431" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="432" spans="1:6" ht="16">
       <c r="A432" s="19"/>
       <c r="B432" s="19"/>
-      <c r="C432" s="14" t="s">
-        <v>1126</v>
+      <c r="C432" s="14">
+        <v>11401136</v>
       </c>
       <c r="D432" s="15" t="s">
-        <v>1121</v>
+        <v>1089</v>
       </c>
       <c r="E432" s="15" t="s">
-        <v>964</v>
-      </c>
-      <c r="F432" s="15"/>
+        <v>936</v>
+      </c>
+      <c r="F432" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="433" spans="1:6" ht="16">
       <c r="A433" s="19"/>
       <c r="B433" s="19"/>
-      <c r="C433" s="14" t="s">
-        <v>1127</v>
+      <c r="C433" s="14">
+        <v>11401137</v>
       </c>
       <c r="D433" s="15" t="s">
-        <v>1122</v>
+        <v>1090</v>
       </c>
       <c r="E433" s="15" t="s">
-        <v>964</v>
-      </c>
-      <c r="F433" s="15"/>
+        <v>936</v>
+      </c>
+      <c r="F433" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="434" spans="1:6" ht="16">
       <c r="A434" s="19"/>
       <c r="B434" s="19"/>
-      <c r="C434" s="14" t="s">
-        <v>1128</v>
+      <c r="C434" s="14">
+        <v>11501238</v>
       </c>
       <c r="D434" s="15" t="s">
-        <v>966</v>
+        <v>937</v>
       </c>
       <c r="E434" s="15" t="s">
-        <v>967</v>
-      </c>
-      <c r="F434" s="15"/>
+        <v>938</v>
+      </c>
+      <c r="F434" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="435" spans="1:6" ht="16">
       <c r="A435" s="19"/>
       <c r="B435" s="19"/>
-      <c r="C435" s="14" t="s">
-        <v>1129</v>
+      <c r="C435" s="14">
+        <v>11501339</v>
       </c>
       <c r="D435" s="15" t="s">
-        <v>969</v>
+        <v>939</v>
       </c>
       <c r="E435" s="15" t="s">
-        <v>970</v>
-      </c>
-      <c r="F435" s="15"/>
+        <v>940</v>
+      </c>
+      <c r="F435" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="436" spans="1:6" ht="16">
       <c r="A436" s="19"/>
       <c r="B436" s="19"/>
-      <c r="C436" s="14" t="s">
-        <v>1130</v>
+      <c r="C436" s="14">
+        <v>11501340</v>
       </c>
       <c r="D436" s="15" t="s">
-        <v>972</v>
+        <v>941</v>
       </c>
       <c r="E436" s="15" t="s">
-        <v>970</v>
-      </c>
-      <c r="F436" s="15"/>
+        <v>940</v>
+      </c>
+      <c r="F436" s="15" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="437" spans="1:6" ht="16">
       <c r="A437" s="19"/>
       <c r="B437" s="19"/>
-      <c r="C437" s="14" t="s">
-        <v>1131</v>
+      <c r="C437" s="14">
+        <v>11501341</v>
       </c>
       <c r="D437" s="15" t="s">
-        <v>974</v>
+        <v>942</v>
       </c>
       <c r="E437" s="15" t="s">
-        <v>970</v>
+        <v>940</v>
       </c>
       <c r="F437" s="15" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="438" spans="1:6" ht="16">
       <c r="A438" s="19"/>
       <c r="B438" s="19"/>
       <c r="C438" s="14" t="s">
-        <v>975</v>
+        <v>943</v>
       </c>
       <c r="D438" s="15" t="s">
-        <v>976</v>
+        <v>944</v>
       </c>
       <c r="E438" s="15" t="s">
-        <v>977</v>
+        <v>945</v>
       </c>
       <c r="F438" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="439" spans="1:6" ht="16">
       <c r="A439" s="19"/>
       <c r="B439" s="19"/>
       <c r="C439" s="14" t="s">
-        <v>979</v>
+        <v>947</v>
       </c>
       <c r="D439" s="15" t="s">
-        <v>980</v>
+        <v>948</v>
       </c>
       <c r="E439" s="15" t="s">
-        <v>977</v>
+        <v>945</v>
       </c>
       <c r="F439" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="440" spans="1:6" ht="16">
       <c r="A440" s="19"/>
       <c r="B440" s="19"/>
       <c r="C440" s="14" t="s">
-        <v>981</v>
+        <v>949</v>
       </c>
       <c r="D440" s="15" t="s">
-        <v>982</v>
+        <v>950</v>
       </c>
       <c r="E440" s="15" t="s">
-        <v>977</v>
+        <v>945</v>
       </c>
       <c r="F440" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="441" spans="1:6" ht="16">
       <c r="A441" s="19"/>
       <c r="B441" s="19"/>
       <c r="C441" s="14" t="s">
-        <v>983</v>
+        <v>951</v>
       </c>
       <c r="D441" s="15" t="s">
-        <v>984</v>
+        <v>952</v>
       </c>
       <c r="E441" s="15" t="s">
-        <v>985</v>
+        <v>953</v>
       </c>
       <c r="F441" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="442" spans="1:6" ht="16">
       <c r="A442" s="19"/>
       <c r="B442" s="19"/>
       <c r="C442" s="14" t="s">
-        <v>986</v>
+        <v>954</v>
       </c>
       <c r="D442" s="15" t="s">
-        <v>987</v>
+        <v>955</v>
       </c>
       <c r="E442" s="15" t="s">
-        <v>985</v>
+        <v>953</v>
       </c>
       <c r="F442" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="443" spans="1:6" ht="16">
       <c r="A443" s="19"/>
       <c r="B443" s="19"/>
       <c r="C443" s="14" t="s">
-        <v>988</v>
+        <v>956</v>
       </c>
       <c r="D443" s="15" t="s">
-        <v>989</v>
+        <v>957</v>
       </c>
       <c r="E443" s="15" t="s">
-        <v>985</v>
+        <v>953</v>
       </c>
       <c r="F443" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="444" spans="1:6" ht="16">
       <c r="A444" s="19"/>
       <c r="B444" s="19"/>
       <c r="C444" s="14" t="s">
-        <v>990</v>
+        <v>958</v>
       </c>
       <c r="D444" s="15" t="s">
-        <v>991</v>
+        <v>959</v>
       </c>
       <c r="E444" s="15" t="s">
-        <v>992</v>
+        <v>960</v>
       </c>
       <c r="F444" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="445" spans="1:6" ht="16">
       <c r="A445" s="19"/>
       <c r="B445" s="19"/>
       <c r="C445" s="14" t="s">
-        <v>993</v>
+        <v>961</v>
       </c>
       <c r="D445" s="15" t="s">
-        <v>994</v>
+        <v>962</v>
       </c>
       <c r="E445" s="15" t="s">
-        <v>992</v>
+        <v>960</v>
       </c>
       <c r="F445" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="446" spans="1:6" ht="16">
       <c r="A446" s="19"/>
       <c r="B446" s="19"/>
       <c r="C446" s="14" t="s">
-        <v>995</v>
+        <v>963</v>
       </c>
       <c r="D446" s="15" t="s">
-        <v>996</v>
+        <v>964</v>
       </c>
       <c r="E446" s="15" t="s">
-        <v>997</v>
+        <v>965</v>
       </c>
       <c r="F446" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="447" spans="1:6" ht="16">
       <c r="A447" s="19"/>
       <c r="B447" s="19"/>
       <c r="C447" s="14" t="s">
-        <v>998</v>
+        <v>966</v>
       </c>
       <c r="D447" s="15" t="s">
-        <v>999</v>
+        <v>967</v>
       </c>
       <c r="E447" s="15" t="s">
-        <v>997</v>
+        <v>965</v>
       </c>
       <c r="F447" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="448" spans="1:6" ht="16">
       <c r="A448" s="19"/>
       <c r="B448" s="19"/>
       <c r="C448" s="14" t="s">
-        <v>1000</v>
+        <v>968</v>
       </c>
       <c r="D448" s="15" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="E448" s="15" t="s">
-        <v>997</v>
+        <v>965</v>
       </c>
       <c r="F448" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="449" spans="1:6" ht="16">
       <c r="A449" s="19"/>
       <c r="B449" s="19"/>
       <c r="C449" s="14" t="s">
-        <v>1002</v>
+        <v>970</v>
       </c>
       <c r="D449" s="15" t="s">
-        <v>1003</v>
+        <v>971</v>
       </c>
       <c r="E449" s="15" t="s">
-        <v>997</v>
+        <v>965</v>
       </c>
       <c r="F449" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="450" spans="1:6" ht="16">
       <c r="A450" s="19"/>
       <c r="B450" s="19"/>
       <c r="C450" s="14" t="s">
-        <v>1004</v>
+        <v>972</v>
       </c>
       <c r="D450" s="15" t="s">
-        <v>1005</v>
+        <v>973</v>
       </c>
       <c r="E450" s="15" t="s">
-        <v>1006</v>
+        <v>974</v>
       </c>
       <c r="F450" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="451" spans="1:6" ht="16">
       <c r="A451" s="19"/>
       <c r="B451" s="19"/>
       <c r="C451" s="14" t="s">
-        <v>1007</v>
+        <v>975</v>
       </c>
       <c r="D451" s="15" t="s">
-        <v>1008</v>
+        <v>976</v>
       </c>
       <c r="E451" s="15" t="s">
-        <v>1006</v>
+        <v>974</v>
       </c>
       <c r="F451" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="452" spans="1:6" ht="16">
       <c r="A452" s="19"/>
       <c r="B452" s="19"/>
       <c r="C452" s="14" t="s">
-        <v>1009</v>
+        <v>977</v>
       </c>
       <c r="D452" s="15" t="s">
-        <v>1010</v>
+        <v>978</v>
       </c>
       <c r="E452" s="15" t="s">
-        <v>1011</v>
+        <v>979</v>
       </c>
       <c r="F452" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="453" spans="1:6" ht="16">
       <c r="A453" s="19"/>
       <c r="B453" s="19"/>
       <c r="C453" s="14" t="s">
-        <v>1012</v>
+        <v>980</v>
       </c>
       <c r="D453" s="15" t="s">
-        <v>1013</v>
+        <v>981</v>
       </c>
       <c r="E453" s="15" t="s">
-        <v>1011</v>
+        <v>979</v>
       </c>
       <c r="F453" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="454" spans="1:6" ht="16">
       <c r="A454" s="19"/>
       <c r="B454" s="19"/>
       <c r="C454" s="14" t="s">
-        <v>1014</v>
+        <v>982</v>
       </c>
       <c r="D454" s="15" t="s">
-        <v>1015</v>
+        <v>983</v>
       </c>
       <c r="E454" s="15" t="s">
-        <v>1016</v>
+        <v>984</v>
       </c>
       <c r="F454" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="455" spans="1:6" ht="16">
       <c r="A455" s="19"/>
       <c r="B455" s="19"/>
       <c r="C455" s="14" t="s">
-        <v>1017</v>
+        <v>985</v>
       </c>
       <c r="D455" s="15" t="s">
-        <v>1018</v>
+        <v>986</v>
       </c>
       <c r="E455" s="15" t="s">
-        <v>1016</v>
+        <v>984</v>
       </c>
       <c r="F455" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="456" spans="1:6" ht="16">
       <c r="A456" s="19"/>
       <c r="B456" s="19"/>
       <c r="C456" s="14" t="s">
-        <v>1019</v>
+        <v>987</v>
       </c>
       <c r="D456" s="15" t="s">
-        <v>1020</v>
+        <v>988</v>
       </c>
       <c r="E456" s="15" t="s">
-        <v>1021</v>
+        <v>989</v>
       </c>
       <c r="F456" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="457" spans="1:6" ht="16">
       <c r="A457" s="19"/>
       <c r="B457" s="19"/>
       <c r="C457" s="14" t="s">
-        <v>1022</v>
+        <v>990</v>
       </c>
       <c r="D457" s="15" t="s">
-        <v>1023</v>
+        <v>991</v>
       </c>
       <c r="E457" s="15" t="s">
-        <v>1021</v>
+        <v>989</v>
       </c>
       <c r="F457" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="458" spans="1:6" ht="16">
       <c r="A458" s="19"/>
       <c r="B458" s="19"/>
       <c r="C458" s="14" t="s">
-        <v>1024</v>
+        <v>992</v>
       </c>
       <c r="D458" s="15" t="s">
-        <v>1025</v>
+        <v>993</v>
       </c>
       <c r="E458" s="15" t="s">
-        <v>1021</v>
+        <v>989</v>
       </c>
       <c r="F458" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="459" spans="1:6" ht="16">
       <c r="A459" s="19"/>
       <c r="B459" s="19"/>
       <c r="C459" s="14" t="s">
-        <v>1026</v>
+        <v>994</v>
       </c>
       <c r="D459" s="15" t="s">
-        <v>1027</v>
+        <v>995</v>
       </c>
       <c r="E459" s="15" t="s">
-        <v>1021</v>
+        <v>989</v>
       </c>
       <c r="F459" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="460" spans="1:6" ht="16">
       <c r="A460" s="19"/>
       <c r="B460" s="19"/>
       <c r="C460" s="14" t="s">
-        <v>1028</v>
+        <v>996</v>
       </c>
       <c r="D460" s="15" t="s">
-        <v>1029</v>
+        <v>997</v>
       </c>
       <c r="E460" s="15" t="s">
-        <v>1030</v>
+        <v>998</v>
       </c>
       <c r="F460" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="461" spans="1:6" ht="16">
       <c r="A461" s="19"/>
       <c r="B461" s="19"/>
       <c r="C461" s="14" t="s">
-        <v>1031</v>
+        <v>999</v>
       </c>
       <c r="D461" s="15" t="s">
-        <v>1032</v>
+        <v>1000</v>
       </c>
       <c r="E461" s="15" t="s">
-        <v>1030</v>
+        <v>998</v>
       </c>
       <c r="F461" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="462" spans="1:6" ht="16">
       <c r="A462" s="19"/>
       <c r="B462" s="19"/>
       <c r="C462" s="14" t="s">
-        <v>1033</v>
+        <v>1001</v>
       </c>
       <c r="D462" s="15" t="s">
-        <v>1034</v>
+        <v>1002</v>
       </c>
       <c r="E462" s="15" t="s">
-        <v>1030</v>
+        <v>998</v>
       </c>
       <c r="F462" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="463" spans="1:6" ht="16">
       <c r="A463" s="19"/>
       <c r="B463" s="19"/>
       <c r="C463" s="14" t="s">
-        <v>1035</v>
+        <v>1003</v>
       </c>
       <c r="D463" s="15" t="s">
-        <v>1036</v>
+        <v>1004</v>
       </c>
       <c r="E463" s="15" t="s">
-        <v>1030</v>
+        <v>998</v>
       </c>
       <c r="F463" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="464" spans="1:6" ht="16">
       <c r="A464" s="19"/>
       <c r="B464" s="19"/>
       <c r="C464" s="14" t="s">
-        <v>1037</v>
+        <v>1005</v>
       </c>
       <c r="D464" s="15" t="s">
-        <v>1038</v>
+        <v>1006</v>
       </c>
       <c r="E464" s="15" t="s">
-        <v>1039</v>
+        <v>1007</v>
       </c>
       <c r="F464" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="465" spans="1:6" ht="16">
       <c r="A465" s="19"/>
       <c r="B465" s="19"/>
       <c r="C465" s="14" t="s">
-        <v>1040</v>
+        <v>1008</v>
       </c>
       <c r="D465" s="15" t="s">
-        <v>1041</v>
+        <v>1009</v>
       </c>
       <c r="E465" s="15" t="s">
-        <v>1039</v>
+        <v>1007</v>
       </c>
       <c r="F465" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="466" spans="1:6" ht="16">
       <c r="A466" s="19"/>
       <c r="B466" s="19"/>
       <c r="C466" s="14" t="s">
-        <v>1042</v>
+        <v>1010</v>
       </c>
       <c r="D466" s="15" t="s">
-        <v>1043</v>
+        <v>1011</v>
       </c>
       <c r="E466" s="15" t="s">
-        <v>1044</v>
+        <v>1012</v>
       </c>
       <c r="F466" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="467" spans="1:6" ht="16">
       <c r="A467" s="19"/>
       <c r="B467" s="19"/>
       <c r="C467" s="14" t="s">
-        <v>1045</v>
+        <v>1013</v>
       </c>
       <c r="D467" s="15" t="s">
-        <v>1046</v>
+        <v>1014</v>
       </c>
       <c r="E467" s="15" t="s">
-        <v>1044</v>
+        <v>1012</v>
       </c>
       <c r="F467" s="15" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
     </row>
     <row r="468" spans="1:6" ht="16">
@@ -17042,10 +16940,10 @@
         <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>1086</v>
+        <v>1054</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>1085</v>
+        <v>1053</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -17122,10 +17020,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>1087</v>
+        <v>1055</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>1088</v>
+        <v>1056</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -17193,7 +17091,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>1089</v>
+        <v>1057</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -17228,7 +17126,7 @@
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="34" t="s">
-        <v>1090</v>
+        <v>1058</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -17262,16 +17160,16 @@
         <v>45</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>1093</v>
+        <v>1061</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>1098</v>
+        <v>1066</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>1100</v>
+        <v>1068</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -17303,16 +17201,16 @@
         <v>51</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>1094</v>
+        <v>1062</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>127</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>1098</v>
+        <v>1066</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>1100</v>
+        <v>1068</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -17343,16 +17241,16 @@
         <v>101</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>1096</v>
+        <v>1064</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>224</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>1098</v>
+        <v>1066</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>1100</v>
+        <v>1068</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -17383,16 +17281,16 @@
         <v>107</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>1095</v>
+        <v>1063</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>238</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>1098</v>
+        <v>1066</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>1100</v>
+        <v>1068</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
@@ -17427,13 +17325,13 @@
         <v>121</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>1097</v>
+        <v>1065</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>1098</v>
+        <v>1066</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>1099</v>
+        <v>1067</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -45861,16 +45759,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1060</v>
+        <v>1028</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1061</v>
+        <v>1029</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1062</v>
+        <v>1030</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1049</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
@@ -45882,10 +45780,10 @@
         <v>25</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>1091</v>
+        <v>1059</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>1104</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
@@ -49940,53 +49838,53 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="22" t="s">
-        <v>1047</v>
+        <v>1015</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>1048</v>
+        <v>1016</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1049</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>1051</v>
+        <v>1019</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>1052</v>
+        <v>1020</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>1053</v>
+        <v>1021</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>1050</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>1054</v>
+        <v>1022</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>1055</v>
+        <v>1023</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>1056</v>
+        <v>1024</v>
       </c>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>1057</v>
+        <v>1025</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>1058</v>
+        <v>1026</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>1059</v>
+        <v>1027</v>
       </c>
       <c r="D4" s="24"/>
     </row>
@@ -55012,22 +54910,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1063</v>
+        <v>1031</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1064</v>
+        <v>1032</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1065</v>
+        <v>1033</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>1066</v>
+        <v>1034</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>1067</v>
+        <v>1035</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1068</v>
+        <v>1036</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -55055,10 +54953,10 @@
         <v>2015</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1092</v>
+        <v>1060</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1084</v>
+        <v>1052</v>
       </c>
       <c r="D2" s="32">
         <v>145</v>
@@ -59113,22 +59011,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1063</v>
+        <v>1031</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1064</v>
+        <v>1032</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1065</v>
+        <v>1033</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>1066</v>
+        <v>1034</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>1067</v>
+        <v>1035</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1068</v>
+        <v>1036</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -59153,13 +59051,13 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="32" t="s">
-        <v>1069</v>
+        <v>1037</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1092</v>
+        <v>1060</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1070</v>
+        <v>1038</v>
       </c>
       <c r="D2" s="32">
         <v>145</v>
@@ -59173,7 +59071,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="32" t="s">
-        <v>1071</v>
+        <v>1039</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -59189,7 +59087,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="32" t="s">
-        <v>1072</v>
+        <v>1040</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -63211,19 +63109,19 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>1073</v>
+        <v>1041</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1074</v>
+        <v>1042</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1075</v>
+        <v>1043</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1076</v>
+        <v>1044</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1077</v>
+        <v>1045</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -63249,7 +63147,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
-        <v>1078</v>
+        <v>1046</v>
       </c>
       <c r="B2" s="5">
         <v>4923</v>
@@ -63267,7 +63165,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>1079</v>
+        <v>1047</v>
       </c>
       <c r="B3" s="5">
         <v>1202</v>
@@ -63285,7 +63183,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>1080</v>
+        <v>1048</v>
       </c>
       <c r="B4" s="5">
         <v>3002</v>
@@ -63303,7 +63201,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>1081</v>
+        <v>1049</v>
       </c>
       <c r="B5" s="5">
         <v>1234</v>
@@ -63321,7 +63219,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>1082</v>
+        <v>1050</v>
       </c>
       <c r="B6" s="5">
         <v>4321</v>
@@ -63339,7 +63237,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>1083</v>
+        <v>1051</v>
       </c>
       <c r="B7" s="5">
         <v>3211</v>

</xml_diff>